<commit_message>
Test Cases filled out.
</commit_message>
<xml_diff>
--- a/Final/TestCase,Bugs,CR Document.xlsx
+++ b/Final/TestCase,Bugs,CR Document.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b855d3120665d134/Documents/Summer 2018/CS 451/Checkers/CS451_Checkers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdesl\OneDrive\Documents\Summer 2018\CS 451\Checkers\CS451_Checkers\Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC8F69E5-031C-4CAD-BB88-EE8EAF153F7C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{AC8F69E5-031C-4CAD-BB88-EE8EAF153F7C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{F3598FD1-D648-4DD4-A0EB-DB45CF340E97}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11150" xr2:uid="{DD82A856-0862-4A98-9F3E-384C8B607037}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="217">
   <si>
     <t>ID</t>
   </si>
@@ -80,9 +80,6 @@
     </r>
   </si>
   <si>
-    <t>GUI window changes to show the hosting game menu. The users IP address is shown. Message states waiting for opponent to join.</t>
-  </si>
-  <si>
     <t>A2</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
   </si>
   <si>
     <t>Join a game</t>
-  </si>
-  <si>
-    <t>GUI window changes to allow user to enter to enter the Host IP Address. Once submitted the GUI window changes to show the user has connected.</t>
   </si>
   <si>
     <t>A3</t>
@@ -197,7 +191,97 @@
     </r>
   </si>
   <si>
-    <t>GUI Window changes to a game board with timer in top right corner and tokens (red in every other square in the first three rows and white in every other square in the last three rows). Players are assigned turns (Player 1 and Player 2). Players are alerted who’s turn it is first.</t>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>R2.1.5</t>
+  </si>
+  <si>
+    <t>Player’s ID is shown.</t>
+  </si>
+  <si>
+    <t>The player’s ID should reflect if they got the first move or second by saying Player 1 or Player 2.</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>R2.1.6</t>
+  </si>
+  <si>
+    <t>Current Player’s Turn is shown.</t>
+  </si>
+  <si>
+    <t>Your player id should be shown above the timer in the top right corner.</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>Player makes a legal move.</t>
+  </si>
+  <si>
+    <t>Token will move to the empty square diagonal to its original position and your turn will end.</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>Player makes an illegal move</t>
+  </si>
+  <si>
+    <t>Token will not move, and you are prompted to make another move selection.</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>Player makes a legal move with a king.</t>
+  </si>
+  <si>
+    <t>King will move to empty square you selected, and your turn ends.</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>Player gets a king token.</t>
+  </si>
+  <si>
+    <t>Token is transformed into a king and your turn ends</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>Player makes a legal jump.</t>
+  </si>
+  <si>
+    <t>Token will jump over opponent token, opponent token that was jumped is removed from the board, and player’s turn ends.</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>Player makes a multi jump</t>
+  </si>
+  <si>
+    <t>The token is moved to the last square in the jump, all opponent tokens that were jumped are removed from the board, and the player’s turn ends.</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>R2.2.5</t>
+  </si>
+  <si>
+    <t>Player request a pause.</t>
   </si>
   <si>
     <r>
@@ -220,102 +304,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Click the Join Game button
-2.       Enter Host IP Address in IP Address Text box and press enter.</t>
-    </r>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>R2.1.5</t>
-  </si>
-  <si>
-    <t>Player’s ID is shown.</t>
-  </si>
-  <si>
-    <t>The player’s ID should reflect if they got the first move or second by saying Player 1 or Player 2.</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>R2.1.6</t>
-  </si>
-  <si>
-    <t>Current Player’s Turn is shown.</t>
-  </si>
-  <si>
-    <t>Your player id should be shown above the timer in the top right corner.</t>
-  </si>
-  <si>
-    <t>B3</t>
-  </si>
-  <si>
-    <t>Player makes a legal move.</t>
-  </si>
-  <si>
-    <t>Token will move to the empty square diagonal to its original position and your turn will end.</t>
-  </si>
-  <si>
-    <t>B4</t>
-  </si>
-  <si>
-    <t>Player makes an illegal move</t>
-  </si>
-  <si>
-    <t>Token will not move, and you are prompted to make another move selection.</t>
-  </si>
-  <si>
-    <t>B5</t>
-  </si>
-  <si>
-    <t>B6</t>
-  </si>
-  <si>
-    <t>B7</t>
-  </si>
-  <si>
-    <t>Player makes a legal move with a king.</t>
-  </si>
-  <si>
-    <t>King will move to empty square you selected, and your turn ends.</t>
-  </si>
-  <si>
-    <t>B8</t>
-  </si>
-  <si>
-    <t>Player gets a king token.</t>
-  </si>
-  <si>
-    <t>Token is transformed into a king and your turn ends</t>
-  </si>
-  <si>
-    <t>B9</t>
-  </si>
-  <si>
-    <t>Player makes a legal jump.</t>
-  </si>
-  <si>
-    <t>Token will jump over opponent token, opponent token that was jumped is removed from the board, and player’s turn ends.</t>
-  </si>
-  <si>
-    <t>B10</t>
-  </si>
-  <si>
-    <t>Player makes a multi jump</t>
-  </si>
-  <si>
-    <t>The token is moved to the last square in the jump, all opponent tokens that were jumped are removed from the board, and the player’s turn ends.</t>
-  </si>
-  <si>
-    <t>B11</t>
-  </si>
-  <si>
-    <t>R2.2.5</t>
-  </si>
-  <si>
-    <t>Player request a pause.</t>
+      <t>Click the pause game button.</t>
+    </r>
+  </si>
+  <si>
+    <t>A pause request is sent to the opponent, the game stops the timer, and the GUI updates saying a pause has been requested.</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>Player request is accepted</t>
   </si>
   <si>
     <r>
@@ -338,17 +337,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Click the pause game button.</t>
-    </r>
-  </si>
-  <si>
-    <t>A pause request is sent to the opponent, the game stops the timer, and the GUI updates saying a pause has been requested.</t>
-  </si>
-  <si>
-    <t>B12</t>
-  </si>
-  <si>
-    <t>Player request is accepted</t>
+      <t>Wait for opponent to accept the pause.</t>
+    </r>
+  </si>
+  <si>
+    <t>The game is paused, and the paused game menu appears.</t>
+  </si>
+  <si>
+    <t>B13</t>
+  </si>
+  <si>
+    <t>Player request is rejected</t>
   </si>
   <si>
     <r>
@@ -371,17 +370,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Wait for opponent to accept the pause.</t>
-    </r>
-  </si>
-  <si>
-    <t>The game is paused, and the paused game menu appears.</t>
-  </si>
-  <si>
-    <t>B13</t>
-  </si>
-  <si>
-    <t>Player request is rejected</t>
+      <t>Wait for opponent to reject the pause request.</t>
+    </r>
+  </si>
+  <si>
+    <t>Your turn resumes, and the pause request menu disappears.</t>
+  </si>
+  <si>
+    <t>B14</t>
+  </si>
+  <si>
+    <t>R2.2.8</t>
+  </si>
+  <si>
+    <t>Player is alerted their turn has begun</t>
   </si>
   <si>
     <r>
@@ -404,47 +406,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Wait for opponent to reject the pause request.</t>
-    </r>
-  </si>
-  <si>
-    <t>Your turn resumes, and the pause request menu disappears.</t>
-  </si>
-  <si>
-    <t>B14</t>
-  </si>
-  <si>
-    <t>R2.2.8</t>
-  </si>
-  <si>
-    <t>Player is alerted their turn has begun</t>
-  </si>
-  <si>
-    <r>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Wait for your opponent to finish their turn.</t>
     </r>
-  </si>
-  <si>
-    <t>A window will appear saying your turn will start. A count down will start. When the countdown ends, the window disappears, the move timer resumes counting down, and the player can click the board and buttons.</t>
   </si>
   <si>
     <t>R2.2.1,
@@ -456,106 +419,6 @@
 R2.2.2,
 R2.2.3,
 R2.2.4</t>
-  </si>
-  <si>
-    <r>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Click on one of your king tokens.
-2.       Click on an empty diagonal square either above or below the king.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Click on a token one row away from the opponents back row.
-2.       Move the token into the opponents back row.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Select a token that is next to an opponent’s token.
-2.       Select the empty square on the other side of the token (must be diagonal to the player and opponent tokens.)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Select a token that is next to an opponent’s token.
-2.       Select the last square in the multi jump. (The square must be diagonal to an opponent’s token and have an empty square diagonal to that opponent that the player could land in form another jumps.)</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">
@@ -869,9 +732,6 @@
     </r>
   </si>
   <si>
-    <t>The game ends Both players are taken to the game over screen and it states you won by capturing all your opponent’s tokens.</t>
-  </si>
-  <si>
     <t>E4</t>
   </si>
   <si>
@@ -924,30 +784,6 @@
   </si>
   <si>
     <t>Exit the game</t>
-  </si>
-  <si>
-    <r>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Click the exit game button on the game over screen.</t>
-    </r>
   </si>
   <si>
     <t>The application closes.</t>
@@ -1161,31 +997,6 @@
 R2.1.4</t>
   </si>
   <si>
-    <r>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Click on one of your tokens.
-2.      Click on an another one of your tokens.</t>
-    </r>
-  </si>
-  <si>
     <t>Bug</t>
   </si>
   <si>
@@ -1341,9 +1152,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Click on one of your tokens.
-2.      Click on an empty square (below your token on the left or right if you are red or above your token on the left or right if you are white.)</t>
-    </r>
+      <t>Click the Join Game button</t>
+    </r>
+  </si>
+  <si>
+    <t>GUI window changes to show game board. The user cannot click on the board or move his pieces until the other player joins.</t>
+  </si>
+  <si>
+    <t>Server menu also opens.</t>
+  </si>
+  <si>
+    <t>GUI window changes to show game board. Player connects to host and the game starts.</t>
+  </si>
+  <si>
+    <t>Not implemented</t>
+  </si>
+  <si>
+    <t>GUI Window changes to a game board with timer in top right corner and tokens (red in every other square in the first three rows and white in every other square in the last three rows). Players are assigned turns (Player 1 and Player 2). Players are alerted who’s turn it currently is by saying not your turn or your turn.</t>
   </si>
   <si>
     <r>
@@ -1367,7 +1192,8 @@
         <scheme val="minor"/>
       </rPr>
       <t>Click on one of your tokens.
-2.      Click on an opponent token.</t>
+2.      Click on an empty square (below your token on the left or right if you are red or above your token on the left or right if you are white.)
+3.     Click the submit button.</t>
     </r>
   </si>
   <si>
@@ -1392,8 +1218,243 @@
         <scheme val="minor"/>
       </rPr>
       <t>Click on one of your tokens.
-2.      Click on an empty square not diagonal to your token.</t>
-    </r>
+2.      Click on an opponent token.
+3.     Click the submit button.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Click on one of your tokens.
+2.      Click on an empty square not diagonal to your token.
+3.     Click the submit button.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Click on one of your tokens.
+2.      Click on an another one of your tokens.
+3.     Click the submit button.</t>
+    </r>
+  </si>
+  <si>
+    <t>Can not select one of your own pieces to begin with so passed but not as expected</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Select a token that is next to an opponent’s token.
+2.       Select the empty square on the other side of the token (must be diagonal to the player and opponent tokens.)
+3.     Click the submit button.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Select a token that is next to an opponent’s token.
+2.       Select the last square in the multi jump. (The square must be diagonal to an opponent’s token and have an empty square diagonal to that opponent that the player could land in form another jumps.)
+3.     Click the submit button.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Click on a token one row away from the opponents back row.
+2.       Move the token into the opponents back row.
+3.     Click the submit button.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Click on one of your king tokens.
+2.       Click on an empty diagonal square either above or below the king.
+3.     Click the submit button.</t>
+    </r>
+  </si>
+  <si>
+    <t>Not your turn message turns into Your turn message.</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Close the application using red x in the top right corner.</t>
+    </r>
+  </si>
+  <si>
+    <t>The game ends, neither player can input moves. Both players Your turn/not your turn messages changes to which player has won (Player 1/2 Wins !!!)</t>
+  </si>
+  <si>
+    <t>As expected, GUI window shows the board and I cannot implement moves.</t>
+  </si>
+  <si>
+    <t>As expected, GUI window shows the board and the game starts.</t>
+  </si>
+  <si>
+    <t>As expected, GUI is displayed correctly and tokens are in the order described.</t>
+  </si>
+  <si>
+    <t>As expected, token moves correctly and buttons work.</t>
+  </si>
+  <si>
+    <t>As expected, token wouldn’t move and I was alerted to retry move.</t>
+  </si>
+  <si>
+    <t>As expected,  token wouldn’t move and I was alerted to retry move.</t>
+  </si>
+  <si>
+    <t>As expected, king can move in any diagonal direction.</t>
+  </si>
+  <si>
+    <t>As expected, token sprite is updated to a king sprite.</t>
+  </si>
+  <si>
+    <t>As expected, token jumped and landed in the right square. Opponent token was removed.</t>
+  </si>
+  <si>
+    <t>As expected, token jumped and landed in the right square. Opponent tokens were removed.</t>
+  </si>
+  <si>
+    <t>As expected, message changes.</t>
+  </si>
+  <si>
+    <t>As expected, move is reflected.</t>
+  </si>
+  <si>
+    <t>As expected, can not move any of my tokens.</t>
+  </si>
+  <si>
+    <t>As expected, message changes and can not make any more moves.</t>
+  </si>
+  <si>
+    <t>As expected, application closes.</t>
   </si>
 </sst>
 </file>
@@ -1564,7 +1625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1632,11 +1693,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="26">
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1751,6 +1835,154 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -1888,6 +2120,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1895,181 +2136,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2094,33 +2160,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7C368C85-B405-41DA-BB20-ED6B6257581E}" name="Table2" displayName="Table2" ref="A1:H37" totalsRowShown="0" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7C368C85-B405-41DA-BB20-ED6B6257581E}" name="Table2" displayName="Table2" ref="A1:H37" totalsRowShown="0" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="A1:H37" xr:uid="{9FC2EB90-F177-44FE-BCC9-A88C6D9A7821}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A852167B-F7C7-45E4-ADBB-407F160F2BC6}" name="ID" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{9F61AA27-59BE-4379-8DA5-A0A98D5AE7D6}" name="Req " dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{0D7310F7-0738-4037-B0E4-BAB18FFEF2C9}" name="Priority" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{CC54D623-2C22-491C-89B6-0BC146B875FB}" name="Description" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{FBB5DA0C-1E37-40E0-B444-7A077D8C229F}" name="Execution Steps" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{8DEB10E5-6213-4BDA-9F83-A9869A107383}" name="Expected Results" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{F7CED197-9E8E-4E72-BE58-154E5F838CCA}" name="Actual Results" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{5E24DF1B-BCBD-41B3-9BD1-7970B0CBF30C}" name="Comments" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{A852167B-F7C7-45E4-ADBB-407F160F2BC6}" name="ID" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{9F61AA27-59BE-4379-8DA5-A0A98D5AE7D6}" name="Req " dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{0D7310F7-0738-4037-B0E4-BAB18FFEF2C9}" name="Priority" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{CC54D623-2C22-491C-89B6-0BC146B875FB}" name="Description" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{FBB5DA0C-1E37-40E0-B444-7A077D8C229F}" name="Execution Steps" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{8DEB10E5-6213-4BDA-9F83-A9869A107383}" name="Expected Results" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{F7CED197-9E8E-4E72-BE58-154E5F838CCA}" name="Actual Results" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{5E24DF1B-BCBD-41B3-9BD1-7970B0CBF30C}" name="Comments" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E749246-301D-4407-9A94-76D54B4BF086}" name="Table1" displayName="Table1" ref="A1:G7" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="24" tableBorderDxfId="25" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E749246-301D-4407-9A94-76D54B4BF086}" name="Table1" displayName="Table1" ref="A1:G7" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="A1:G7" xr:uid="{71BE82F1-23FB-4A33-A95B-8FB4B6168CD4}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{151A6730-8107-4579-9F81-7A436CCE8927}" name="ID" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{37E52CAD-3253-459C-B226-61685DA8C5CA}" name="Severity" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{4F05236F-0F11-437D-83BD-92DF1F5D7A95}" name="Priority" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{39E0E654-1EF4-4965-B935-5C9B5780085F}" name="Bug" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{731DE1C1-369E-4A26-9FCA-84787219F9C5}" name="Fix" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{71D7395F-01E2-453E-96DB-F64A97DAD087}" name="Release Version" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{D8B74241-F39A-4033-A62A-DC97CAC26B3F}" name="CRs" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{151A6730-8107-4579-9F81-7A436CCE8927}" name="ID" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{37E52CAD-3253-459C-B226-61685DA8C5CA}" name="Severity" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{4F05236F-0F11-437D-83BD-92DF1F5D7A95}" name="Priority" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{39E0E654-1EF4-4965-B935-5C9B5780085F}" name="Bug" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{731DE1C1-369E-4A26-9FCA-84787219F9C5}" name="Fix" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{71D7395F-01E2-453E-96DB-F64A97DAD087}" name="Release Version" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{D8B74241-F39A-4033-A62A-DC97CAC26B3F}" name="CRs" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2130,10 +2196,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{810C04FB-C220-4390-871E-4226D15686E3}" name="Table3" displayName="Table3" ref="A1:D7" totalsRowShown="0">
   <autoFilter ref="A1:D7" xr:uid="{2858AD64-E9B1-4C41-A617-65584BB03CFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CE6BE018-72F3-4898-92B0-8760F1361F3F}" name="CR" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{FDB67E9E-111B-470F-AC1D-E68D6242AAD9}" name="Version Released On" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{B7E05CB3-23E0-49B9-9797-2946A8A3C853}" name="Reason For Change" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{CED59BD0-35C7-48EC-AB10-21191AD2557F}" name="Approval" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{CE6BE018-72F3-4898-92B0-8760F1361F3F}" name="CR" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{FDB67E9E-111B-470F-AC1D-E68D6242AAD9}" name="Version Released On" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{B7E05CB3-23E0-49B9-9797-2946A8A3C853}" name="Reason For Change" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{CED59BD0-35C7-48EC-AB10-21191AD2557F}" name="Approval" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2438,8 +2504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EC41ED-28FB-4F4A-A53D-166F45459AD1}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
+      <selection activeCell="G41" sqref="G40:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2450,7 +2516,7 @@
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="60" style="5" customWidth="1"/>
     <col min="6" max="6" width="64.81640625" customWidth="1"/>
-    <col min="7" max="7" width="26.08984375" customWidth="1"/>
+    <col min="7" max="7" width="26.08984375" style="30" customWidth="1"/>
     <col min="8" max="8" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2474,13 +2540,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -2497,779 +2563,853 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C3" s="6">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>184</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>187</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="7">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="7">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="3"/>
+        <v>189</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>204</v>
+      </c>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C7" s="8">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C8" s="8">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>205</v>
+      </c>
       <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C10" s="6">
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>206</v>
+      </c>
       <c r="H10" s="11"/>
     </row>
     <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C11" s="6">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>207</v>
+      </c>
       <c r="H11" s="11"/>
     </row>
     <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C12" s="6">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="11"/>
-    </row>
-    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
-        <v>46</v>
-      </c>
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C13" s="6">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>78</v>
+        <v>198</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>208</v>
+      </c>
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C14" s="6">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>79</v>
+        <v>197</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>209</v>
+      </c>
       <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C15" s="6">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>80</v>
+        <v>195</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>210</v>
+      </c>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C16" s="6">
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>81</v>
+        <v>196</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>211</v>
+      </c>
       <c r="H16" s="11"/>
     </row>
     <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C17" s="8">
         <v>2</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C18" s="8">
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G18" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C19" s="8">
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C20" s="8">
         <v>2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" s="3"/>
+        <v>199</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>212</v>
+      </c>
       <c r="H20" s="11"/>
     </row>
     <row r="21" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C21" s="6">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G21" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>213</v>
+      </c>
       <c r="H21" s="11"/>
     </row>
     <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C22" s="8">
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H22" s="11"/>
     </row>
     <row r="23" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C23" s="8">
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G23" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="19" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C24" s="6">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G24" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>214</v>
+      </c>
       <c r="H24" s="11"/>
     </row>
     <row r="25" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C25" s="8">
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G25" s="3"/>
+        <v>99</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H25" s="11"/>
     </row>
     <row r="26" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C26" s="8">
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G26" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H26" s="11"/>
     </row>
     <row r="27" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="19" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C27" s="8">
         <v>2</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G27" s="3"/>
+        <v>105</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H27" s="11"/>
     </row>
     <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="19" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C28" s="7">
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G28" s="3"/>
+        <v>109</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H28" s="11"/>
     </row>
     <row r="29" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="19" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C29" s="7">
         <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G29" s="3"/>
+        <v>149</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H29" s="11"/>
     </row>
     <row r="30" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="19" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C30" s="6">
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G30" s="3"/>
+        <v>201</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>215</v>
+      </c>
       <c r="H30" s="11"/>
     </row>
     <row r="31" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="19" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C31" s="8">
         <v>2</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G31" s="3"/>
+        <v>119</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H31" s="11"/>
     </row>
     <row r="32" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A32" s="19" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C32" s="7">
         <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G32" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H32" s="11"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C33" s="6">
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>138</v>
+        <v>200</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G33" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>216</v>
+      </c>
       <c r="H33" s="11"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C34" s="6">
-        <v>1</v>
+        <v>130</v>
+      </c>
+      <c r="C34" s="8">
+        <v>2</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G34" s="3"/>
+        <v>133</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H34" s="11"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="19" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="C35" s="8">
         <v>2</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G35" s="3"/>
+        <v>137</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H35" s="11"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="19" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="C36" s="8">
         <v>2</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G36" s="3"/>
+        <v>141</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H36" s="11"/>
     </row>
     <row r="37" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="26" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C37" s="28">
         <v>2</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="F37" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="G37" s="16"/>
+        <v>146</v>
+      </c>
+      <c r="G37" s="29" t="s">
+        <v>188</v>
+      </c>
       <c r="H37" s="18"/>
     </row>
   </sheetData>
@@ -3303,22 +3443,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -3328,10 +3468,10 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="F2" s="3">
         <v>1.1000000000000001</v>
@@ -3347,10 +3487,10 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="F3" s="3">
         <v>1.2</v>
@@ -3366,10 +3506,10 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="2" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="F4" s="3">
         <v>1.3</v>
@@ -3385,10 +3525,10 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="2" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="F5" s="3">
         <v>1.4</v>
@@ -3404,10 +3544,10 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="2" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="F6" s="3">
         <v>1.5</v>
@@ -3423,10 +3563,10 @@
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="17" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="F7" s="16">
         <v>1.6</v>
@@ -3460,16 +3600,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="D1" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -3480,10 +3620,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -3494,10 +3634,10 @@
         <v>1.2</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -3508,10 +3648,10 @@
         <v>1.3</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -3522,10 +3662,10 @@
         <v>1.4</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -3536,10 +3676,10 @@
         <v>1.5</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -3550,10 +3690,10 @@
         <v>1.6</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>